<commit_message>
Updated scraper and file managemet
</commit_message>
<xml_diff>
--- a/backend/data/rankings/game_matchups.xlsx
+++ b/backend/data/rankings/game_matchups.xlsx
@@ -1,43 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8403595d4321e36a/Documents/School/SeniorProject/backend/data/rankings/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_4A7A4D4FC04942CEE838B0764CA62EB8A67E82EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F4F6782-FCB3-4534-8DC0-8E56B65F031B}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rams @ bengals" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="rams @ bengals" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>bengals</t>
+  </si>
+  <si>
+    <t>rams</t>
+  </si>
+  <si>
+    <t>offense</t>
+  </si>
+  <si>
+    <t>defense</t>
+  </si>
+  <si>
+    <t>First Downs Gained By Passing</t>
+  </si>
+  <si>
+    <t>Passing Yards</t>
+  </si>
+  <si>
+    <t>First Downs By Rushing</t>
+  </si>
+  <si>
+    <t>Rushing Plays</t>
+  </si>
+  <si>
+    <t>Rushing Yards</t>
+  </si>
+  <si>
+    <t>Scoring</t>
+  </si>
+  <si>
+    <t>Total Yards</t>
+  </si>
+  <si>
+    <t>Sacks</t>
+  </si>
+  <si>
+    <t>Completion Percentage</t>
+  </si>
+  <si>
+    <t>Turnovers</t>
+  </si>
+  <si>
+    <t>3rd Down Percentage</t>
+  </si>
+  <si>
+    <t>4th Down Percentage</t>
+  </si>
+  <si>
+    <t>Yards Per Completion</t>
+  </si>
+  <si>
+    <t>Yards Per Carry</t>
+  </si>
+  <si>
+    <t>Yards Per Play</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,114 +114,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,339 +441,296 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>bengals</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>rams</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr"/>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>offense</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>defense</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>offense</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>defense</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>First Downs Gained By Passing</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>7</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>32</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>30</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Passing Yards</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>32</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>30</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>First Downs By Rushing</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>21</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>18</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>17</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Rushing Plays</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>13</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>24</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Rushing Yards</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>19</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>19</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>10</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Scoring</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>23</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>21</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Total Yards</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>31</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>3</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>29</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Sacks</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>7</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>24</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>3</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Completion Percentage</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>22</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>6</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>14</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Turnovers</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>11</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>11</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>3</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>3rd Down Percentage</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>21</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>11</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>4th Down Percentage</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>22</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>15</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Yards Per Completion</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>11</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Yards Per Carry</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
         <v>26</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>24</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>29</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>4</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Yards Per Play</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
         <v>8</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>23</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>6</v>
       </c>
     </row>

</xml_diff>